<commit_message>
Added missing index files to 10x pbmc sheet.
</commit_message>
<xml_diff>
--- a/2018-01/SmartSeq2/Q4DemoSS2Metadata_VALID.xlsx
+++ b/2018-01/SmartSeq2/Q4DemoSS2Metadata_VALID.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="3060" windowWidth="25600" windowHeight="13860" activeTab="4"/>
+    <workbookView xWindow="2440" yWindow="3060" windowWidth="25600" windowHeight="13860"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -667,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -926,7 +926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>